<commit_message>
Added totals column for cel/for/pot
</commit_message>
<xml_diff>
--- a/Clanless Card Stats.xlsx
+++ b/Clanless Card Stats.xlsx
@@ -47,7 +47,7 @@
     <t xml:space="preserve">X</t>
   </si>
   <si>
-    <t xml:space="preserve">“4+”</t>
+    <t xml:space="preserve">4+</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -261,6 +261,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -485,10 +486,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E23"/>
+  <dimension ref="A2:F23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -540,6 +541,10 @@
         <f aca="false">COUNTIF(Potence!C1:C30, "="&amp;A4)</f>
         <v>0</v>
       </c>
+      <c r="F4" s="2" t="n">
+        <f aca="false">SUM(B4:E4)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -561,6 +566,10 @@
         <f aca="false">COUNTIF(Potence!C1:C30, "="&amp;A5)</f>
         <v>2</v>
       </c>
+      <c r="F5" s="2" t="n">
+        <f aca="false">SUM(B5:E5)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -582,6 +591,10 @@
         <f aca="false">COUNTIF(Potence!C1:C30, "="&amp;A6)</f>
         <v>6</v>
       </c>
+      <c r="F6" s="2" t="n">
+        <f aca="false">SUM(B6:E6)</f>
+        <v>30</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -603,6 +616,10 @@
         <f aca="false">COUNTIF(Potence!C1:C30, "="&amp;A7)</f>
         <v>4</v>
       </c>
+      <c r="F7" s="2" t="n">
+        <f aca="false">SUM(B7:E7)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -624,6 +641,10 @@
         <f aca="false">COUNTIF(Potence!C1:C30, "="&amp;A8)</f>
         <v>2</v>
       </c>
+      <c r="F8" s="2" t="n">
+        <f aca="false">SUM(B8:E8)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -645,6 +666,10 @@
         <f aca="false">COUNTIF(Potence!C1:C30, "&gt;3")</f>
         <v>0</v>
       </c>
+      <c r="F9" s="2" t="n">
+        <f aca="false">SUM(B9:E9)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -666,11 +691,16 @@
         <f aca="false">SUM(E4:E9)</f>
         <v>14</v>
       </c>
+      <c r="F10" s="2" t="n">
+        <f aca="false">SUM(B10:E10)</f>
+        <v>52</v>
+      </c>
     </row>
     <row r="12" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
@@ -692,6 +722,10 @@
         <f aca="false">COUNTIF(Potence!B1:B30, "=Attack")</f>
         <v>10</v>
       </c>
+      <c r="F13" s="2" t="n">
+        <f aca="false">SUM(B13:E13)</f>
+        <v>21</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
@@ -713,6 +747,10 @@
         <f aca="false">COUNTIF(Potence!B1:B30, "=Skill")</f>
         <v>2</v>
       </c>
+      <c r="F14" s="2" t="n">
+        <f aca="false">SUM(B14:E14)</f>
+        <v>22</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
@@ -734,6 +772,10 @@
         <f aca="false">COUNTIF(Potence!B1:B30, "=Power")</f>
         <v>2</v>
       </c>
+      <c r="F15" s="2" t="n">
+        <f aca="false">SUM(B15:E15)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -755,6 +797,10 @@
         <f aca="false">SUM(E13:E15)</f>
         <v>14</v>
       </c>
+      <c r="F16" s="2" t="n">
+        <f aca="false">SUM(B16:E16)</f>
+        <v>52</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -781,6 +827,10 @@
         <f aca="false">COUNTIF(Potence!D1:D30, "="&amp;A19)</f>
         <v>0</v>
       </c>
+      <c r="F19" s="2" t="n">
+        <f aca="false">SUM(B19:E19)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
@@ -802,6 +852,10 @@
         <f aca="false">COUNTIF(Potence!D1:D30, "="&amp;A20)</f>
         <v>4</v>
       </c>
+      <c r="F20" s="2" t="n">
+        <f aca="false">SUM(B20:E20)</f>
+        <v>16</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
@@ -823,6 +877,10 @@
         <f aca="false">COUNTIF(Potence!D1:D30, "="&amp;A21)</f>
         <v>4</v>
       </c>
+      <c r="F21" s="2" t="n">
+        <f aca="false">SUM(B21:E21)</f>
+        <v>18</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
@@ -844,6 +902,10 @@
         <f aca="false">COUNTIF(Potence!D1:D30, "="&amp;A22)</f>
         <v>6</v>
       </c>
+      <c r="F22" s="2" t="n">
+        <f aca="false">SUM(B22:E22)</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
@@ -864,6 +926,10 @@
       <c r="E23" s="3" t="n">
         <f aca="false">SUM(E19:E22)</f>
         <v>14</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <f aca="false">SUM(B23:E23)</f>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -890,7 +956,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="27.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="27.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="8.61"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="9" width="11.52"/>
@@ -1123,7 +1189,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1307,7 +1373,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1491,7 +1557,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1717,7 +1783,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Fixed auto count formulae.
Added Ablative Skin to the Fortitude sheet.
</commit_message>
<xml_diff>
--- a/Clanless Card Stats.xlsx
+++ b/Clanless Card Stats.xlsx
@@ -489,7 +489,7 @@
   <dimension ref="A2:F23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -526,19 +526,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="n">
-        <f aca="false">COUNTIF(Core!C1:C30, "="&amp;A4)</f>
+        <f aca="false">COUNTIF(Core!$C:$C, "="&amp;$A4)</f>
         <v>0</v>
       </c>
       <c r="C4" s="2" t="n">
-        <f aca="false">COUNTIF(Celerity!C1:C30, "="&amp;A4)</f>
+        <f aca="false">COUNTIF(Celerity!$C:$C, "="&amp;$A4)</f>
         <v>0</v>
       </c>
       <c r="D4" s="2" t="n">
-        <f aca="false">COUNTIF(Fortitude!C1:C30, "="&amp;A4)</f>
+        <f aca="false">COUNTIF(Fortitude!$C:$C, "="&amp;$A4)</f>
         <v>1</v>
       </c>
       <c r="E4" s="2" t="n">
-        <f aca="false">COUNTIF(Potence!C1:C30, "="&amp;A4)</f>
+        <f aca="false">COUNTIF(Potence!$C:$C, "="&amp;$A4)</f>
         <v>0</v>
       </c>
       <c r="F4" s="2" t="n">
@@ -550,20 +550,20 @@
       <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="3" t="n">
-        <f aca="false">COUNTIF(Core!C1:C30, "="&amp;A5)</f>
+      <c r="B5" s="2" t="n">
+        <f aca="false">COUNTIF(Core!$C:$C, "="&amp;$A5)</f>
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="n">
-        <f aca="false">COUNTIF(Celerity!C1:C30, "="&amp;A5)</f>
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <f aca="false">COUNTIF(Fortitude!C1:C30, "="&amp;A5)</f>
+      <c r="C5" s="2" t="n">
+        <f aca="false">COUNTIF(Celerity!$C:$C, "="&amp;$A5)</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <f aca="false">COUNTIF(Fortitude!$C:$C, "="&amp;$A5)</f>
         <v>3</v>
       </c>
-      <c r="E5" s="3" t="n">
-        <f aca="false">COUNTIF(Potence!C1:C30, "="&amp;A5)</f>
+      <c r="E5" s="2" t="n">
+        <f aca="false">COUNTIF(Potence!$C:$C, "="&amp;$A5)</f>
         <v>2</v>
       </c>
       <c r="F5" s="2" t="n">
@@ -575,20 +575,20 @@
       <c r="A6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B6" s="3" t="n">
-        <f aca="false">COUNTIF(Core!C1:C30, "="&amp;A6)</f>
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <f aca="false">COUNTIF(Celerity!C1:C30, "="&amp;A6)</f>
+      <c r="B6" s="2" t="n">
+        <f aca="false">COUNTIF(Core!$C:$C, "="&amp;$A6)</f>
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <f aca="false">COUNTIF(Celerity!$C:$C, "="&amp;$A6)</f>
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="n">
-        <f aca="false">COUNTIF(Fortitude!C1:C30, "="&amp;A6)</f>
+      <c r="D6" s="2" t="n">
+        <f aca="false">COUNTIF(Fortitude!$C:$C, "="&amp;$A6)</f>
         <v>5</v>
       </c>
-      <c r="E6" s="3" t="n">
-        <f aca="false">COUNTIF(Potence!C1:C30, "="&amp;A6)</f>
+      <c r="E6" s="2" t="n">
+        <f aca="false">COUNTIF(Potence!$C:$C, "="&amp;$A6)</f>
         <v>6</v>
       </c>
       <c r="F6" s="2" t="n">
@@ -600,20 +600,20 @@
       <c r="A7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="n">
-        <f aca="false">COUNTIF(Core!C1:C30, "="&amp;A7)</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="3" t="n">
-        <f aca="false">COUNTIF(Celerity!C1:C30, "="&amp;A7)</f>
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="n">
-        <f aca="false">COUNTIF(Fortitude!C1:C30, "="&amp;A7)</f>
-        <v>2</v>
-      </c>
-      <c r="E7" s="3" t="n">
-        <f aca="false">COUNTIF(Potence!C1:C30, "="&amp;A7)</f>
+      <c r="B7" s="2" t="n">
+        <f aca="false">COUNTIF(Core!$C:$C, "="&amp;$A7)</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <f aca="false">COUNTIF(Celerity!$C:$C, "="&amp;$A7)</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <f aca="false">COUNTIF(Fortitude!$C:$C, "="&amp;$A7)</f>
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <f aca="false">COUNTIF(Potence!$C:$C, "="&amp;$A7)</f>
         <v>4</v>
       </c>
       <c r="F7" s="2" t="n">
@@ -625,20 +625,20 @@
       <c r="A8" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B8" s="3" t="n">
-        <f aca="false">COUNTIF(Core!C1:C30, "="&amp;A8)</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="3" t="n">
-        <f aca="false">COUNTIF(Celerity!C1:C30, "="&amp;A8)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <f aca="false">COUNTIF(Fortitude!C1:C30, "="&amp;A8)</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="3" t="n">
-        <f aca="false">COUNTIF(Potence!C1:C30, "="&amp;A8)</f>
+      <c r="B8" s="2" t="n">
+        <f aca="false">COUNTIF(Core!$C:$C, "="&amp;$A8)</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <f aca="false">COUNTIF(Celerity!$C:$C, "="&amp;$A8)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <f aca="false">COUNTIF(Fortitude!$C:$C, "="&amp;$A8)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <f aca="false">COUNTIF(Potence!$C:$C, "="&amp;$A8)</f>
         <v>2</v>
       </c>
       <c r="F8" s="2" t="n">
@@ -650,20 +650,20 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="n">
-        <f aca="false">COUNTIF(Core!C1:C30, "&gt;3")</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="3" t="n">
-        <f aca="false">COUNTIF(Celerity!C1:C30, "&gt;3")</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="3" t="n">
-        <f aca="false">COUNTIF(Fortitude!C1:C30, "&gt;3")</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="3" t="n">
-        <f aca="false">COUNTIF(Potence!C1:C30, "&gt;3")</f>
+      <c r="B9" s="2" t="n">
+        <f aca="false">COUNTIF(Core!$C:$C, "&gt;3")</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <f aca="false">COUNTIF(Celerity!$C:$C, "&gt;3")</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <f aca="false">COUNTIF(Fortitude!$C:$C, "&gt;3")</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <f aca="false">COUNTIF(Potence!$C:$C, "&gt;3")</f>
         <v>0</v>
       </c>
       <c r="F9" s="2" t="n">
@@ -707,19 +707,19 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="n">
-        <f aca="false">COUNTIF(Core!B1:B30, "=Attack")</f>
+        <f aca="false">COUNTIF(Core!$B:$B, "="&amp;$A13)</f>
         <v>8</v>
       </c>
-      <c r="C13" s="3" t="n">
-        <f aca="false">COUNTIF(Celerity!B1:B30, "=Attack")</f>
-        <v>2</v>
-      </c>
-      <c r="D13" s="3" t="n">
-        <f aca="false">COUNTIF(Fortitude!B1:B30, "=Attack")</f>
-        <v>1</v>
-      </c>
-      <c r="E13" s="3" t="n">
-        <f aca="false">COUNTIF(Potence!B1:B30, "=Attack")</f>
+      <c r="C13" s="2" t="n">
+        <f aca="false">COUNTIF(Celerity!$B:$B, "="&amp;$A13)</f>
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <f aca="false">COUNTIF(Fortitude!$B:$B, "="&amp;$A13)</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <f aca="false">COUNTIF(Potence!$B:$B, "="&amp;$A13)</f>
         <v>10</v>
       </c>
       <c r="F13" s="2" t="n">
@@ -732,19 +732,19 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="n">
-        <f aca="false">COUNTIF(Core!B1:B30, "=Skill")</f>
+        <f aca="false">COUNTIF(Core!$B:$B, "="&amp;$A14)</f>
         <v>7</v>
       </c>
-      <c r="C14" s="3" t="n">
-        <f aca="false">COUNTIF(Celerity!B1:B30, "=Skill")</f>
+      <c r="C14" s="2" t="n">
+        <f aca="false">COUNTIF(Celerity!$B:$B, "="&amp;$A14)</f>
         <v>7</v>
       </c>
-      <c r="D14" s="3" t="n">
-        <f aca="false">COUNTIF(Fortitude!B1:B30, "=Skill")</f>
+      <c r="D14" s="2" t="n">
+        <f aca="false">COUNTIF(Fortitude!$B:$B, "="&amp;$A14)</f>
         <v>6</v>
       </c>
-      <c r="E14" s="3" t="n">
-        <f aca="false">COUNTIF(Potence!B1:B30, "=Skill")</f>
+      <c r="E14" s="2" t="n">
+        <f aca="false">COUNTIF(Potence!$B:$B, "="&amp;$A14)</f>
         <v>2</v>
       </c>
       <c r="F14" s="2" t="n">
@@ -757,19 +757,19 @@
         <v>12</v>
       </c>
       <c r="B15" s="2" t="n">
-        <f aca="false">COUNTIF(Core!B1:B30, "=Power")</f>
-        <v>1</v>
-      </c>
-      <c r="C15" s="3" t="n">
-        <f aca="false">COUNTIF(Celerity!B1:B30, "=Power")</f>
-        <v>2</v>
-      </c>
-      <c r="D15" s="3" t="n">
-        <f aca="false">COUNTIF(Fortitude!B1:B30, "=Power")</f>
+        <f aca="false">COUNTIF(Core!$B:$B, "="&amp;$A15)</f>
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <f aca="false">COUNTIF(Celerity!$B:$B, "="&amp;$A15)</f>
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <f aca="false">COUNTIF(Fortitude!$B:$B, "="&amp;$A15)</f>
         <v>4</v>
       </c>
-      <c r="E15" s="3" t="n">
-        <f aca="false">COUNTIF(Potence!B1:B30, "=Power")</f>
+      <c r="E15" s="2" t="n">
+        <f aca="false">COUNTIF(Potence!$B:$B, "="&amp;$A15)</f>
         <v>2</v>
       </c>
       <c r="F15" s="2" t="n">
@@ -812,19 +812,19 @@
         <v>14</v>
       </c>
       <c r="B19" s="2" t="n">
-        <f aca="false">COUNTIF(Core!D1:D30, "="&amp;A19)</f>
+        <f aca="false">COUNTIF(Core!$D:$D, "="&amp;$A19)</f>
         <v>4</v>
       </c>
-      <c r="C19" s="3" t="n">
-        <f aca="false">COUNTIF(Celerity!D1:D30, "="&amp;B19)</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="3" t="n">
-        <f aca="false">COUNTIF(Fortitude!D1:D30, "="&amp;A19)</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="3" t="n">
-        <f aca="false">COUNTIF(Potence!D1:D30, "="&amp;A19)</f>
+      <c r="C19" s="2" t="n">
+        <f aca="false">COUNTIF(Celerity!$D:$D, "="&amp;$A19)</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <f aca="false">COUNTIF(Fortitude!$D:$D, "="&amp;$A19)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <f aca="false">COUNTIF(Potence!$D:$D, "="&amp;$A19)</f>
         <v>0</v>
       </c>
       <c r="F19" s="2" t="n">
@@ -836,20 +836,20 @@
       <c r="A20" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="3" t="n">
-        <f aca="false">COUNTIF(Core!D1:D30, "="&amp;A20)</f>
+      <c r="B20" s="2" t="n">
+        <f aca="false">COUNTIF(Core!$D:$D, "="&amp;$A20)</f>
         <v>6</v>
       </c>
-      <c r="C20" s="3" t="n">
-        <f aca="false">COUNTIF(Celerity!D1:D30, "="&amp;A20)</f>
-        <v>2</v>
-      </c>
-      <c r="D20" s="3" t="n">
-        <f aca="false">COUNTIF(Fortitude!D1:D30, "="&amp;A20)</f>
+      <c r="C20" s="2" t="n">
+        <f aca="false">COUNTIF(Celerity!$D:$D, "="&amp;$A20)</f>
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <f aca="false">COUNTIF(Fortitude!$D:$D, "="&amp;$A20)</f>
         <v>4</v>
       </c>
-      <c r="E20" s="3" t="n">
-        <f aca="false">COUNTIF(Potence!D1:D30, "="&amp;A20)</f>
+      <c r="E20" s="2" t="n">
+        <f aca="false">COUNTIF(Potence!$D:$D, "="&amp;$A20)</f>
         <v>4</v>
       </c>
       <c r="F20" s="2" t="n">
@@ -861,20 +861,20 @@
       <c r="A21" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="3" t="n">
-        <f aca="false">COUNTIF(Core!D3:D32, "="&amp;A21)</f>
+      <c r="B21" s="2" t="n">
+        <f aca="false">COUNTIF(Core!$D:$D, "="&amp;$A21)</f>
         <v>4</v>
       </c>
-      <c r="C21" s="3" t="n">
-        <f aca="false">COUNTIF(Celerity!D1:D30, "="&amp;A21)</f>
+      <c r="C21" s="2" t="n">
+        <f aca="false">COUNTIF(Celerity!$D:$D, "="&amp;$A21)</f>
         <v>6</v>
       </c>
-      <c r="D21" s="3" t="n">
-        <f aca="false">COUNTIF(Fortitude!D1:D30, "="&amp;A21)</f>
+      <c r="D21" s="2" t="n">
+        <f aca="false">COUNTIF(Fortitude!$D:$D, "="&amp;$A21)</f>
         <v>4</v>
       </c>
-      <c r="E21" s="3" t="n">
-        <f aca="false">COUNTIF(Potence!D1:D30, "="&amp;A21)</f>
+      <c r="E21" s="2" t="n">
+        <f aca="false">COUNTIF(Potence!$D:$D, "="&amp;$A21)</f>
         <v>4</v>
       </c>
       <c r="F21" s="2" t="n">
@@ -886,20 +886,20 @@
       <c r="A22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="3" t="n">
-        <f aca="false">COUNTIF(Core!D1:D30, "="&amp;A22)</f>
-        <v>2</v>
-      </c>
-      <c r="C22" s="3" t="n">
-        <f aca="false">COUNTIF(Celerity!D1:D30, "="&amp;A22)</f>
+      <c r="B22" s="2" t="n">
+        <f aca="false">COUNTIF(Core!$D:$D, "="&amp;$A22)</f>
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <f aca="false">COUNTIF(Celerity!$D:$D, "="&amp;$A22)</f>
         <v>3</v>
       </c>
-      <c r="D22" s="3" t="n">
-        <f aca="false">COUNTIF(Fortitude!D1:D30, "="&amp;A22)</f>
+      <c r="D22" s="2" t="n">
+        <f aca="false">COUNTIF(Fortitude!$D:$D, "="&amp;$A22)</f>
         <v>3</v>
       </c>
-      <c r="E22" s="3" t="n">
-        <f aca="false">COUNTIF(Potence!D1:D30, "="&amp;A22)</f>
+      <c r="E22" s="2" t="n">
+        <f aca="false">COUNTIF(Potence!$D:$D, "="&amp;$A22)</f>
         <v>6</v>
       </c>
       <c r="F22" s="2" t="n">

</xml_diff>

<commit_message>
Updated card list spreadsheet.
</commit_message>
<xml_diff>
--- a/Clanless Card Stats.xlsx
+++ b/Clanless Card Stats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="79">
   <si>
     <t xml:space="preserve">Energy Distribution</t>
   </si>
@@ -161,6 +161,12 @@
     <t xml:space="preserve">Infernal Pursuit</t>
   </si>
   <si>
+    <t xml:space="preserve">Lightning Reflexes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mercury’s Arrow</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nimble Feet</t>
   </si>
   <si>
@@ -173,6 +179,9 @@
     <t xml:space="preserve">Vampiric Speed</t>
   </si>
   <si>
+    <t xml:space="preserve">Ablative Skin</t>
+  </si>
+  <si>
     <t xml:space="preserve">Daring the Dawn</t>
   </si>
   <si>
@@ -218,6 +227,9 @@
     <t xml:space="preserve">Fists of Death</t>
   </si>
   <si>
+    <t xml:space="preserve">Forger’s Hammer</t>
+  </si>
+  <si>
     <t xml:space="preserve">Growing Fury</t>
   </si>
   <si>
@@ -228,6 +240,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mighty Grapple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pushing the Limit</t>
   </si>
   <si>
     <t xml:space="preserve">Shattering Blow</t>
@@ -488,8 +503,8 @@
   </sheetPr>
   <dimension ref="A2:F23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -531,7 +546,7 @@
       </c>
       <c r="C4" s="2" t="n">
         <f aca="false">COUNTIF(Celerity!$C:$C, "="&amp;$A4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$C:$C, "="&amp;$A4)</f>
@@ -543,7 +558,7 @@
       </c>
       <c r="F4" s="2" t="n">
         <f aca="false">SUM(B4:E4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -581,7 +596,7 @@
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">COUNTIF(Celerity!$C:$C, "="&amp;$A6)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$C:$C, "="&amp;$A6)</f>
@@ -589,11 +604,11 @@
       </c>
       <c r="E6" s="2" t="n">
         <f aca="false">COUNTIF(Potence!$C:$C, "="&amp;$A6)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F6" s="2" t="n">
         <f aca="false">SUM(B6:E6)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -610,15 +625,15 @@
       </c>
       <c r="D7" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$C:$C, "="&amp;$A7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="2" t="n">
         <f aca="false">COUNTIF(Potence!$C:$C, "="&amp;$A7)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7" s="2" t="n">
         <f aca="false">SUM(B7:E7)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -681,19 +696,19 @@
       </c>
       <c r="C10" s="2" t="n">
         <f aca="false">SUM(C4:C9)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2" t="n">
         <f aca="false">SUM(D4:D9)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" s="3" t="n">
         <f aca="false">SUM(E4:E9)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F10" s="2" t="n">
         <f aca="false">SUM(B10:E10)</f>
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,7 +727,7 @@
       </c>
       <c r="C13" s="2" t="n">
         <f aca="false">COUNTIF(Celerity!$B:$B, "="&amp;$A13)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$B:$B, "="&amp;$A13)</f>
@@ -720,11 +735,11 @@
       </c>
       <c r="E13" s="2" t="n">
         <f aca="false">COUNTIF(Potence!$B:$B, "="&amp;$A13)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F13" s="2" t="n">
         <f aca="false">SUM(B13:E13)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -737,7 +752,7 @@
       </c>
       <c r="C14" s="2" t="n">
         <f aca="false">COUNTIF(Celerity!$B:$B, "="&amp;$A14)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$B:$B, "="&amp;$A14)</f>
@@ -745,11 +760,11 @@
       </c>
       <c r="E14" s="2" t="n">
         <f aca="false">COUNTIF(Potence!$B:$B, "="&amp;$A14)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" s="2" t="n">
         <f aca="false">SUM(B14:E14)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -766,7 +781,7 @@
       </c>
       <c r="D15" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$B:$B, "="&amp;$A15)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E15" s="2" t="n">
         <f aca="false">COUNTIF(Potence!$B:$B, "="&amp;$A15)</f>
@@ -774,7 +789,7 @@
       </c>
       <c r="F15" s="2" t="n">
         <f aca="false">SUM(B15:E15)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,19 +802,19 @@
       </c>
       <c r="C16" s="3" t="n">
         <f aca="false">SUM(C13:C15)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D16" s="3" t="n">
         <f aca="false">SUM(D13:D15)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" s="3" t="n">
         <f aca="false">SUM(E13:E15)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F16" s="2" t="n">
         <f aca="false">SUM(B16:E16)</f>
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,7 +857,7 @@
       </c>
       <c r="C20" s="2" t="n">
         <f aca="false">COUNTIF(Celerity!$D:$D, "="&amp;$A20)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$D:$D, "="&amp;$A20)</f>
@@ -850,11 +865,11 @@
       </c>
       <c r="E20" s="2" t="n">
         <f aca="false">COUNTIF(Potence!$D:$D, "="&amp;$A20)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F20" s="2" t="n">
         <f aca="false">SUM(B20:E20)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -871,15 +886,15 @@
       </c>
       <c r="D21" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$D:$D, "="&amp;$A21)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E21" s="2" t="n">
         <f aca="false">COUNTIF(Potence!$D:$D, "="&amp;$A21)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F21" s="2" t="n">
         <f aca="false">SUM(B21:E21)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -892,7 +907,7 @@
       </c>
       <c r="C22" s="2" t="n">
         <f aca="false">COUNTIF(Celerity!$D:$D, "="&amp;$A22)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D22" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$D:$D, "="&amp;$A22)</f>
@@ -904,7 +919,7 @@
       </c>
       <c r="F22" s="2" t="n">
         <f aca="false">SUM(B22:E22)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -917,19 +932,19 @@
       </c>
       <c r="C23" s="3" t="n">
         <f aca="false">SUM(C19:C22)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D23" s="3" t="n">
         <f aca="false">SUM(D19:D22)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E23" s="3" t="n">
         <f aca="false">SUM(E19:E22)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F23" s="2" t="n">
         <f aca="false">SUM(B23:E23)</f>
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1202,15 +1217,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="16.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="10" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="9" width="11.52"/>
@@ -1321,11 +1336,11 @@
       <c r="B8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="10" t="n">
-        <v>1</v>
+      <c r="C8" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1333,13 +1348,13 @@
         <v>46</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1347,7 +1362,7 @@
         <v>47</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="10" t="n">
         <v>1</v>
@@ -1367,6 +1382,34 @@
         <v>1</v>
       </c>
       <c r="D11" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1386,10 +1429,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1402,80 +1445,80 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C1" s="10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>6</v>
+      <c r="C4" s="10" t="n">
+        <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="10" t="n">
-        <v>0</v>
+      <c r="C5" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="10" t="n">
         <v>0</v>
@@ -1486,41 +1529,41 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>28</v>
@@ -1528,7 +1571,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>12</v>
@@ -1537,20 +1580,34 @@
         <v>1</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1570,10 +1627,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1586,7 +1643,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>10</v>
@@ -1600,7 +1657,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>10</v>
@@ -1614,7 +1671,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>11</v>
@@ -1628,7 +1685,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>12</v>
@@ -1642,27 +1699,27 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>34</v>
@@ -1670,35 +1727,35 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="10" t="n">
         <v>2</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" s="10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>10</v>
@@ -1707,18 +1764,18 @@
         <v>1</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>19</v>
@@ -1726,27 +1783,27 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>19</v>
@@ -1754,29 +1811,57 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Fleetness and Precision.
Cleaned up redundant keyword strings.

Gave Thrown Gate and Thrown Sewer Lid the RANGED flag.
</commit_message>
<xml_diff>
--- a/Clanless Card Stats.xlsx
+++ b/Clanless Card Stats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="84">
   <si>
     <t xml:space="preserve">Energy Distribution</t>
   </si>
@@ -56,6 +56,9 @@
     <t xml:space="preserve">Type Distribution</t>
   </si>
   <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Attack</t>
   </si>
   <si>
@@ -68,6 +71,9 @@
     <t xml:space="preserve">Rarity Distribution</t>
   </si>
   <si>
+    <t xml:space="preserve">Rarity</t>
+  </si>
+  <si>
     <t xml:space="preserve">Starter</t>
   </si>
   <si>
@@ -158,6 +164,9 @@
     <t xml:space="preserve">Flash</t>
   </si>
   <si>
+    <t xml:space="preserve">Fleetness</t>
+  </si>
+  <si>
     <t xml:space="preserve">Infernal Pursuit</t>
   </si>
   <si>
@@ -168,6 +177,9 @@
   </si>
   <si>
     <t xml:space="preserve">Nimble Feet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precision</t>
   </si>
   <si>
     <t xml:space="preserve">Psyche!</t>
@@ -504,20 +516,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:F23"/>
+  <dimension ref="A2:F25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="2" width="10.41"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="2" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="2" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,7 +611,7 @@
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">COUNTIF(Celerity!$C:$C, "="&amp;$A6)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$C:$C, "="&amp;$A6)</f>
@@ -611,7 +623,7 @@
       </c>
       <c r="F6" s="2" t="n">
         <f aca="false">SUM(B6:E6)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -624,7 +636,7 @@
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">COUNTIF(Celerity!$C:$C, "="&amp;$A7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$C:$C, "="&amp;$A7)</f>
@@ -636,7 +648,7 @@
       </c>
       <c r="F7" s="2" t="n">
         <f aca="false">SUM(B7:E7)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -699,7 +711,7 @@
       </c>
       <c r="C10" s="2" t="n">
         <f aca="false">SUM(C4:C9)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2" t="n">
         <f aca="false">SUM(D4:D9)</f>
@@ -711,59 +723,51 @@
       </c>
       <c r="F10" s="2" t="n">
         <f aca="false">SUM(B10:E10)</f>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+    <row r="13" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="2" t="n">
-        <f aca="false">COUNTIF(Core!$B:$B, "="&amp;$A13)</f>
-        <v>8</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <f aca="false">COUNTIF(Celerity!$B:$B, "="&amp;$A13)</f>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="2" t="n">
-        <f aca="false">COUNTIF(Fortitude!$B:$B, "="&amp;$A13)</f>
-        <v>2</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <f aca="false">COUNTIF(Potence!$B:$B, "="&amp;$A13)</f>
-        <v>11</v>
-      </c>
-      <c r="F13" s="2" t="n">
-        <f aca="false">SUM(B13:E13)</f>
-        <v>24</v>
+      <c r="D13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="2" t="n">
         <f aca="false">COUNTIF(Core!$B:$B, "="&amp;$A14)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" s="2" t="n">
         <f aca="false">COUNTIF(Celerity!$B:$B, "="&amp;$A14)</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D14" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$B:$B, "="&amp;$A14)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E14" s="2" t="n">
         <f aca="false">COUNTIF(Potence!$B:$B, "="&amp;$A14)</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F14" s="2" t="n">
         <f aca="false">SUM(B14:E14)</f>
@@ -771,112 +775,108 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="2" t="n">
         <f aca="false">COUNTIF(Core!$B:$B, "="&amp;$A15)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2" t="n">
         <f aca="false">COUNTIF(Celerity!$B:$B, "="&amp;$A15)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D15" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$B:$B, "="&amp;$A15)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E15" s="2" t="n">
         <f aca="false">COUNTIF(Potence!$B:$B, "="&amp;$A15)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" s="2" t="n">
         <f aca="false">SUM(B15:E15)</f>
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>8</v>
+      <c r="A16" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="B16" s="2" t="n">
-        <f aca="false">SUM(B13:B15)</f>
-        <v>16</v>
-      </c>
-      <c r="C16" s="3" t="n">
-        <f aca="false">SUM(C13:C15)</f>
-        <v>13</v>
-      </c>
-      <c r="D16" s="3" t="n">
-        <f aca="false">SUM(D13:D15)</f>
-        <v>13</v>
-      </c>
-      <c r="E16" s="3" t="n">
-        <f aca="false">SUM(E13:E15)</f>
-        <v>16</v>
+        <f aca="false">COUNTIF(Core!$B:$B, "="&amp;$A16)</f>
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <f aca="false">COUNTIF(Celerity!$B:$B, "="&amp;$A16)</f>
+        <v>4</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <f aca="false">COUNTIF(Fortitude!$B:$B, "="&amp;$A16)</f>
+        <v>5</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <f aca="false">COUNTIF(Potence!$B:$B, "="&amp;$A16)</f>
+        <v>2</v>
       </c>
       <c r="F16" s="2" t="n">
         <f aca="false">SUM(B16:E16)</f>
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <f aca="false">SUM(B14:B16)</f>
+        <v>16</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <f aca="false">SUM(C14:C16)</f>
+        <v>15</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <f aca="false">SUM(D14:D16)</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="3" t="n">
+        <f aca="false">SUM(E14:E16)</f>
+        <v>16</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <f aca="false">SUM(B17:E17)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="2" t="n">
-        <f aca="false">COUNTIF(Core!$D:$D, "="&amp;$A19)</f>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="2" t="n">
-        <f aca="false">COUNTIF(Celerity!$D:$D, "="&amp;$A19)</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <f aca="false">COUNTIF(Fortitude!$D:$D, "="&amp;$A19)</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="n">
-        <f aca="false">COUNTIF(Potence!$D:$D, "="&amp;$A19)</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="2" t="n">
-        <f aca="false">SUM(B19:E19)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="2" t="n">
-        <f aca="false">COUNTIF(Core!$D:$D, "="&amp;$A20)</f>
-        <v>6</v>
-      </c>
-      <c r="C20" s="2" t="n">
-        <f aca="false">COUNTIF(Celerity!$D:$D, "="&amp;$A20)</f>
-        <v>3</v>
-      </c>
-      <c r="D20" s="2" t="n">
-        <f aca="false">COUNTIF(Fortitude!$D:$D, "="&amp;$A20)</f>
-        <v>4</v>
-      </c>
-      <c r="E20" s="2" t="n">
-        <f aca="false">COUNTIF(Potence!$D:$D, "="&amp;$A20)</f>
+      <c r="E20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="2" t="n">
-        <f aca="false">SUM(B20:E20)</f>
-        <v>18</v>
-      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="2" t="n">
@@ -885,32 +885,32 @@
       </c>
       <c r="C21" s="2" t="n">
         <f aca="false">COUNTIF(Celerity!$D:$D, "="&amp;$A21)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$D:$D, "="&amp;$A21)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E21" s="2" t="n">
         <f aca="false">COUNTIF(Potence!$D:$D, "="&amp;$A21)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F21" s="2" t="n">
         <f aca="false">SUM(B21:E21)</f>
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="2" t="n">
         <f aca="false">COUNTIF(Core!$D:$D, "="&amp;$A22)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2" t="n">
         <f aca="false">COUNTIF(Celerity!$D:$D, "="&amp;$A22)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D22" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$D:$D, "="&amp;$A22)</f>
@@ -918,39 +918,94 @@
       </c>
       <c r="E22" s="2" t="n">
         <f aca="false">COUNTIF(Potence!$D:$D, "="&amp;$A22)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F22" s="2" t="n">
         <f aca="false">SUM(B22:E22)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <f aca="false">COUNTIF(Core!$D:$D, "="&amp;$A23)</f>
+        <v>4</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <f aca="false">COUNTIF(Celerity!$D:$D, "="&amp;$A23)</f>
         <v>8</v>
       </c>
-      <c r="B23" s="2" t="n">
-        <f aca="false">SUM(B19:B22)</f>
-        <v>16</v>
-      </c>
-      <c r="C23" s="3" t="n">
-        <f aca="false">SUM(C19:C22)</f>
-        <v>13</v>
-      </c>
-      <c r="D23" s="3" t="n">
-        <f aca="false">SUM(D19:D22)</f>
-        <v>13</v>
-      </c>
-      <c r="E23" s="3" t="n">
-        <f aca="false">SUM(E19:E22)</f>
-        <v>16</v>
+      <c r="D23" s="2" t="n">
+        <f aca="false">COUNTIF(Fortitude!$D:$D, "="&amp;$A23)</f>
+        <v>5</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <f aca="false">COUNTIF(Potence!$D:$D, "="&amp;$A23)</f>
+        <v>5</v>
       </c>
       <c r="F23" s="2" t="n">
         <f aca="false">SUM(B23:E23)</f>
-        <v>58</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <f aca="false">COUNTIF(Core!$D:$D, "="&amp;$A24)</f>
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <f aca="false">COUNTIF(Celerity!$D:$D, "="&amp;$A24)</f>
+        <v>4</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <f aca="false">COUNTIF(Fortitude!$D:$D, "="&amp;$A24)</f>
+        <v>4</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <f aca="false">COUNTIF(Potence!$D:$D, "="&amp;$A24)</f>
+        <v>6</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <f aca="false">SUM(B24:E24)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="2" t="n">
+        <f aca="false">SUM(B21:B24)</f>
+        <v>16</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <f aca="false">SUM(C21:C24)</f>
+        <v>15</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <f aca="false">SUM(D21:D24)</f>
+        <v>13</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <f aca="false">SUM(E21:E24)</f>
+        <v>16</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <f aca="false">SUM(B25:E25)</f>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A19:E19"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -982,226 +1037,226 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1220,10 +1275,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1236,133 +1291,133 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="10" t="n">
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="10" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>1</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="10" t="n">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>11</v>
@@ -1371,49 +1426,77 @@
         <v>1</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>28</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1448,184 +1531,184 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" s="10" t="n">
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="10" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="10" t="n">
         <v>2</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="10" t="n">
         <v>2</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1660,226 +1743,226 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="10" t="n">
         <v>3</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="10" t="n">
         <v>2</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="10" t="n">
         <v>2</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" s="10" t="n">
         <v>2</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="10" t="n">
         <v>2</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="10" t="n">
         <v>2</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" s="10" t="n">
         <v>3</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Armor of Vitality!
</commit_message>
<xml_diff>
--- a/Clanless Card Stats.xlsx
+++ b/Clanless Card Stats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="86">
   <si>
     <t xml:space="preserve">Energy Distribution</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ablative Skin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armor of Vitality</t>
   </si>
   <si>
     <t xml:space="preserve">Daring the Dawn</t>
@@ -526,7 +529,7 @@
   <dimension ref="A2:F25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -626,7 +629,7 @@
       </c>
       <c r="D6" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$C:$C, "="&amp;$A6)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" s="2" t="n">
         <f aca="false">COUNTIF(Potence!$C:$C, "="&amp;$A6)</f>
@@ -634,7 +637,7 @@
       </c>
       <c r="F6" s="2" t="n">
         <f aca="false">SUM(B6:E6)</f>
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -726,7 +729,7 @@
       </c>
       <c r="D10" s="2" t="n">
         <f aca="false">SUM(D4:D9)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E10" s="4" t="n">
         <f aca="false">SUM(E4:E9)</f>
@@ -734,7 +737,7 @@
       </c>
       <c r="F10" s="2" t="n">
         <f aca="false">SUM(B10:E10)</f>
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -803,7 +806,7 @@
       </c>
       <c r="D15" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$B:$B, "="&amp;$A15)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E15" s="2" t="n">
         <f aca="false">COUNTIF(Potence!$B:$B, "="&amp;$A15)</f>
@@ -811,7 +814,7 @@
       </c>
       <c r="F15" s="2" t="n">
         <f aca="false">SUM(B15:E15)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,7 +856,7 @@
       </c>
       <c r="D17" s="4" t="n">
         <f aca="false">SUM(D14:D16)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E17" s="4" t="n">
         <f aca="false">SUM(E14:E16)</f>
@@ -861,7 +864,7 @@
       </c>
       <c r="F17" s="2" t="n">
         <f aca="false">SUM(B17:E17)</f>
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -954,7 +957,7 @@
       </c>
       <c r="D23" s="2" t="n">
         <f aca="false">COUNTIF(Fortitude!$D:$D, "="&amp;$A23)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E23" s="2" t="n">
         <f aca="false">COUNTIF(Potence!$D:$D, "="&amp;$A23)</f>
@@ -962,7 +965,7 @@
       </c>
       <c r="F23" s="2" t="n">
         <f aca="false">SUM(B23:E23)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1004,7 +1007,7 @@
       </c>
       <c r="D25" s="4" t="n">
         <f aca="false">SUM(D21:D24)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E25" s="4" t="n">
         <f aca="false">SUM(E21:E24)</f>
@@ -1012,7 +1015,7 @@
       </c>
       <c r="F25" s="2" t="n">
         <f aca="false">SUM(B25:E25)</f>
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1292,7 +1295,7 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -1544,10 +1547,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1577,13 +1580,13 @@
         <v>57</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="11" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1591,13 +1594,13 @@
         <v>58</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1605,7 +1608,7 @@
         <v>59</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="11" t="n">
         <v>2</v>
@@ -1619,13 +1622,13 @@
         <v>60</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1635,11 +1638,11 @@
       <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>6</v>
+      <c r="C6" s="11" t="n">
+        <v>1</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1649,11 +1652,11 @@
       <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="11" t="n">
-        <v>0</v>
+      <c r="C7" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1661,7 +1664,7 @@
         <v>63</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="11" t="n">
         <v>0</v>
@@ -1675,13 +1678,13 @@
         <v>64</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" s="11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,10 +1695,10 @@
         <v>12</v>
       </c>
       <c r="C10" s="11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,10 +1706,10 @@
         <v>66</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>30</v>
@@ -1723,7 +1726,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,12 +1734,26 @@
         <v>68</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1772,7 +1789,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>11</v>
@@ -1786,7 +1803,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>11</v>
@@ -1800,7 +1817,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>12</v>
@@ -1814,7 +1831,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>13</v>
@@ -1828,7 +1845,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>12</v>
@@ -1842,7 +1859,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>11</v>
@@ -1856,7 +1873,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>11</v>
@@ -1870,7 +1887,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>13</v>
@@ -1884,7 +1901,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>11</v>
@@ -1898,7 +1915,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>11</v>
@@ -1912,7 +1929,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>11</v>
@@ -1926,7 +1943,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>11</v>
@@ -1940,7 +1957,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -1954,7 +1971,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>12</v>
@@ -1968,7 +1985,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>11</v>
@@ -1982,7 +1999,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>11</v>

</xml_diff>